<commit_message>
Autocalibration now works: respects min and maxs, based on type of transition parameter. Phew! Also includes diary/ script and spreadsheets for running autocalibration on simple cascade.
</commit_message>
<xml_diff>
--- a/data/cascade-simple-calibration.xlsx
+++ b/data/cascade-simple-calibration.xlsx
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E14"/>
+      <selection activeCell="E5" sqref="E5:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1378,9 +1378,7 @@
       <c r="D3" s="7">
         <v>0.02</v>
       </c>
-      <c r="E3" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E3" s="11"/>
       <c r="G3" s="2">
         <v>2</v>
       </c>
@@ -1400,9 +1398,7 @@
       <c r="D4" s="7">
         <v>0.01</v>
       </c>
-      <c r="E4" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E4" s="11"/>
       <c r="G4" s="2">
         <v>2</v>
       </c>
@@ -1475,9 +1471,7 @@
       <c r="D8" s="7">
         <v>0.01</v>
       </c>
-      <c r="E8" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E8" s="11"/>
       <c r="G8" s="2">
         <v>3</v>
       </c>
@@ -1510,9 +1504,7 @@
       <c r="D10" s="7">
         <v>0.01</v>
       </c>
-      <c r="E10" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E10" s="11"/>
       <c r="G10" s="2">
         <v>3</v>
       </c>
@@ -1530,9 +1522,7 @@
       <c r="D11" s="7">
         <v>0.01</v>
       </c>
-      <c r="E11" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="2" t="s">
         <v>92</v>
       </c>
@@ -1550,9 +1540,7 @@
       <c r="D12" s="7">
         <v>0.01</v>
       </c>
-      <c r="E12" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1567,9 +1555,7 @@
       <c r="D13" s="7">
         <v>0.01</v>
       </c>
-      <c r="E13" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1584,9 +1570,7 @@
       <c r="D14" s="7">
         <v>0.01</v>
       </c>
-      <c r="E14" s="11">
-        <v>-1</v>
-      </c>
+      <c r="E14" s="11"/>
       <c r="F14" s="2" t="s">
         <v>92</v>
       </c>
@@ -1619,7 +1603,9 @@
       <c r="D16" s="7">
         <v>100</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11">
+        <v>-1</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Rescales initial compartment values during autofitting.
Note that the step sizes for altering compartments are applied as
factors rather than additive step sizes (this can be improved). 

As a necessity, compartment sizes are only altered for characteristics
that have entry_point values associated with them. To prevent people
disappearing (or being randomly created), characteristics now also has a
'Calibrate?' column (as for the link parameters cascade values) and
entry points associated with total population (e.g. alive = all people,
with susceptible compartment as an entry point) is recommended as a "do
not calibrate this compartment".

An example databook is supplied, with the target link parameters and
initial compartments is also supplied. 

Note that autofit is still fragile - it requires a decent starting value
and can get stuck on "bad" solutions, but it is now useable.
</commit_message>
<xml_diff>
--- a/data/cascade-simple-calibration.xlsx
+++ b/data/cascade-simple-calibration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5420" yWindow="-21800" windowWidth="36160" windowHeight="20120" activeTab="3"/>
+    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
   <si>
     <t>Code Label</t>
   </si>
@@ -398,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -421,12 +421,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -445,9 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,14 +480,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -771,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1036,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1048,14 +1082,14 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="2"/>
+    <col min="5" max="6" width="14.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,231 +1106,258 @@
         <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="14"/>
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="6"/>
+      <c r="K2" s="7"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="14"/>
+      <c r="H3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="G4" s="7" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="14"/>
+      <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="12">
         <v>10000</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="14"/>
+      <c r="H5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="7" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="14"/>
+      <c r="H6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="12">
         <v>200000</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="14">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="2" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="K9" s="10"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="K10" s="19"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1307,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1359,7 +1420,7 @@
       <c r="D2" s="7">
         <v>0.01</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="10"/>
       <c r="G2" s="2">
         <v>1</v>
       </c>
@@ -1378,7 +1439,7 @@
       <c r="D3" s="7">
         <v>0.02</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="10"/>
       <c r="G3" s="2">
         <v>2</v>
       </c>
@@ -1398,7 +1459,7 @@
       <c r="D4" s="7">
         <v>0.01</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
       <c r="G4" s="2">
         <v>2</v>
       </c>
@@ -1417,7 +1478,7 @@
       <c r="D5" s="7">
         <v>0.01</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10"/>
       <c r="G5" s="2">
         <v>4</v>
       </c>
@@ -1435,7 +1496,7 @@
       <c r="D6" s="7">
         <v>0.01</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="10"/>
       <c r="G6" s="2">
         <v>4</v>
       </c>
@@ -1453,7 +1514,7 @@
       <c r="D7" s="7">
         <v>0.01</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="2" t="s">
         <v>94</v>
       </c>
@@ -1471,7 +1532,7 @@
       <c r="D8" s="7">
         <v>0.01</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="10"/>
       <c r="G8" s="2">
         <v>3</v>
       </c>
@@ -1489,7 +1550,7 @@
       <c r="D9" s="7">
         <v>0.01</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1504,7 +1565,7 @@
       <c r="D10" s="7">
         <v>0.01</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="10"/>
       <c r="G10" s="2">
         <v>3</v>
       </c>
@@ -1522,7 +1583,7 @@
       <c r="D11" s="7">
         <v>0.01</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="2" t="s">
         <v>92</v>
       </c>
@@ -1540,7 +1601,7 @@
       <c r="D12" s="7">
         <v>0.01</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1555,7 +1616,7 @@
       <c r="D13" s="7">
         <v>0.01</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1570,7 +1631,7 @@
       <c r="D14" s="7">
         <v>0.01</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="2" t="s">
         <v>92</v>
       </c>
@@ -1588,7 +1649,7 @@
       <c r="D15" s="7">
         <v>0.01</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1603,7 +1664,7 @@
       <c r="D16" s="7">
         <v>100</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">

</xml_diff>